<commit_message>
Update cost calculations and add portfolio cost breakdown
</commit_message>
<xml_diff>
--- a/Cost comparaison 250915.xlsx
+++ b/Cost comparaison 250915.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11214"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/40b27aa5a8b78a75/EPFL/MA3/PdS2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="8_{F3A81C2A-F09B-074C-B822-6B184396A76F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{839B58A4-E655-384F-BAFD-AE77CED304B2}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="8_{F3A81C2A-F09B-074C-B822-6B184396A76F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{46A53CDC-E1F7-374E-9DBC-70A73C30F4E5}"/>
   <bookViews>
     <workbookView xWindow="4320" yWindow="620" windowWidth="24480" windowHeight="17380" xr2:uid="{71B643D5-27B6-F94A-95BE-84F6C9C29DB4}"/>
   </bookViews>
@@ -15911,13 +15911,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DCB1949-3A77-A14C-B817-3F033FDA9505}">
   <dimension ref="A1:N111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="J37" sqref="J37"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="20.6640625" customWidth="1"/>
+    <col min="4" max="4" width="24.5" customWidth="1"/>
     <col min="5" max="5" width="12.83203125" customWidth="1"/>
     <col min="6" max="6" width="12.33203125" customWidth="1"/>
     <col min="12" max="12" width="12.1640625" bestFit="1" customWidth="1"/>

</xml_diff>